<commit_message>
edit PROF_to_WHPE and PIG_to_WHPE fix CTD match up and remove longest common string in STNNBR
I had to change the CTD match up section to check that matches by station number were true in position and time. This had to be fixed because where PIG STNNBR were different to PROF STNNBR, but both were numeric mismatched were occurring
I also added code to both PIG_to_WHPE and PROF_to_WHPE to remove the longest common forward substring from STNNBRS within a cruise.
</commit_message>
<xml_diff>
--- a/product_data/processing_metadata/C4/PROF_meta.xlsx
+++ b/product_data/processing_metadata/C4/PROF_meta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/kimberlee_baldry_utas_edu_au/Documents/Documents/Projects/BIO-MATE/BIO-MATE.v0/processing_metadata/C4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/kimberlee_baldry_utas_edu_au/Documents/Documents/Projects/BIO-MATE/BIO-MATE/product_data/processing_metadata/C4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{EEE577D7-02F7-48DE-BFA1-A7A142926E74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E394A531-AAF1-4E53-BCF8-3A3BCB6F6112}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{EEE577D7-02F7-48DE-BFA1-A7A142926E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E394A531-AAF1-4E53-BCF8-3A3BCB6F6112}"/>
   <bookViews>
-    <workbookView xWindow="32415" yWindow="2145" windowWidth="19770" windowHeight="11940" xr2:uid="{64B97871-A170-45B4-A294-5AEA4BC0E271}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{64B97871-A170-45B4-A294-5AEA4BC0E271}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -897,7 +897,7 @@
   <dimension ref="A1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>